<commit_message>
Got spreadsheets updated to manuscript tables
</commit_message>
<xml_diff>
--- a/LacTissue_hptoolbox.xlsx
+++ b/LacTissue_hptoolbox.xlsx
@@ -2,22 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE4E288-4B82-4140-8BD2-439FCE2205B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD640A53-1C2D-47F5-B6D4-5E8A2FDCF078}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20D85B12-9758-4F64-8529-8B10498F4544}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{20D85B12-9758-4F64-8529-8B10498F4544}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="kpl t test" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="kLefflux t test" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="8" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="73">
   <si>
     <t>Normal</t>
   </si>
@@ -122,6 +123,138 @@
   </si>
   <si>
     <t>kLEfflux</t>
+  </si>
+  <si>
+    <t>1.58E-03</t>
+  </si>
+  <si>
+    <t>1.85E-03</t>
+  </si>
+  <si>
+    <t>4.09E-04</t>
+  </si>
+  <si>
+    <t>1.04E-03</t>
+  </si>
+  <si>
+    <t>1.17E-03</t>
+  </si>
+  <si>
+    <t>9.77E-05</t>
+  </si>
+  <si>
+    <t>7.24E-05</t>
+  </si>
+  <si>
+    <t>8.21E+08</t>
+  </si>
+  <si>
+    <t>8.85E+08</t>
+  </si>
+  <si>
+    <t>2.81E+08</t>
+  </si>
+  <si>
+    <t>1.50E+08</t>
+  </si>
+  <si>
+    <t>1.33E+08</t>
+  </si>
+  <si>
+    <t>1.20E+08</t>
+  </si>
+  <si>
+    <t>4.47E-04</t>
+  </si>
+  <si>
+    <t>1.88E-03</t>
+  </si>
+  <si>
+    <t>2.49E-03</t>
+  </si>
+  <si>
+    <t>1.45E-07</t>
+  </si>
+  <si>
+    <t>1.64E-03</t>
+  </si>
+  <si>
+    <t>1.44E-04</t>
+  </si>
+  <si>
+    <t>8.32E-05</t>
+  </si>
+  <si>
+    <t>3.39E-04</t>
+  </si>
+  <si>
+    <t>6.50E-03</t>
+  </si>
+  <si>
+    <t>1.45E-03</t>
+  </si>
+  <si>
+    <t>1.98E-03</t>
+  </si>
+  <si>
+    <t>0.02 ± 1.44E-04</t>
+  </si>
+  <si>
+    <t>0.02 ± 8.32E-05</t>
+  </si>
+  <si>
+    <t>0.02 ± 3.39E-04</t>
+  </si>
+  <si>
+    <t>0.49 ± 0.02</t>
+  </si>
+  <si>
+    <t>0.62 ± 0.03</t>
+  </si>
+  <si>
+    <t>0.32 ± 0.18</t>
+  </si>
+  <si>
+    <t>4.47E-04 ± 1.45E-07</t>
+  </si>
+  <si>
+    <t>1.88E-03 ± 1.64E-03</t>
+  </si>
+  <si>
+    <t>2.49E-03 ± 2.49E-03</t>
+  </si>
+  <si>
+    <t>0.03 ± 0.01</t>
+  </si>
+  <si>
+    <t>0.03 ± 7.24E-05</t>
+  </si>
+  <si>
+    <t>8.21E+08 ± 1.50E+08</t>
+  </si>
+  <si>
+    <t>21.67 ± 0.99</t>
+  </si>
+  <si>
+    <t>71.99 ± 1.36</t>
+  </si>
+  <si>
+    <t>8.85E+08 ± 1.33E+08</t>
+  </si>
+  <si>
+    <t>23.26 ± 3.55</t>
+  </si>
+  <si>
+    <t>69.93 ± 1.77</t>
+  </si>
+  <si>
+    <t>2.81E+08 ± 1.20E+08</t>
+  </si>
+  <si>
+    <t>17.16 ± 2.67</t>
+  </si>
+  <si>
+    <t>66.51 ± 1.03</t>
   </si>
 </sst>
 </file>
@@ -230,7 +363,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -243,6 +376,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2429,25 +2565,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B8402E-36A7-41FF-A256-45E2644B1621}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="S89" sqref="S89:X89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="18" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>2.8219214062879053E-4</v>
       </c>
@@ -2504,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>4.738731868732241E-3</v>
       </c>
@@ -2561,7 +2698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4.714109952254986E-4</v>
       </c>
@@ -2618,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>6.9029981860676019E-4</v>
       </c>
@@ -2675,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>6.5256505609614783E-4</v>
       </c>
@@ -2766,7 +2903,7 @@
         <v>1.9607843137254902E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4.1234186015919115E-4</v>
       </c>
@@ -2853,7 +2990,7 @@
         <v>2.1276595744680851E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1.8289349482574239E-3</v>
       </c>
@@ -2910,7 +3047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7.4960223764231736E-3</v>
       </c>
@@ -2967,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2.2207063174650723E-3</v>
       </c>
@@ -3024,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2.077569128187533E-4</v>
       </c>
@@ -3081,7 +3218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2.5585370046212586E-4</v>
       </c>
@@ -3138,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3.9688978895393006E-4</v>
       </c>
@@ -3195,7 +3332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>5.1368495621184293E-4</v>
       </c>
@@ -3252,7 +3389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>1.3105383229876472E-2</v>
       </c>
@@ -3309,7 +3446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>3.1190215825482111E-4</v>
       </c>
@@ -3366,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>1.8848694713137994E-4</v>
       </c>
@@ -3423,7 +3560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>1.7887046238220031E-3</v>
       </c>
@@ -3480,7 +3617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>6.2264851846212279E-4</v>
       </c>
@@ -3537,7 +3674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ref="A19:A35" si="1">IF(OR(ABS(A2-T$5)&lt;=0.001*T$5,ABS(A2-T$6)&lt;=0.001*T$6),0,1)</f>
         <v>1</v>
@@ -3575,7 +3712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3613,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3651,7 +3788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3689,7 +3826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3727,7 +3864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3771,7 +3908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3818,7 +3955,7 @@
         <v>1.8538458865264319E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3862,7 +3999,7 @@
         <v>1.1694195702938643E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3900,7 +4037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3938,7 +4075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3976,7 +4113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4020,7 +4157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4067,7 +4204,7 @@
         <v>0.7489205966313609</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4111,7 +4248,7 @@
         <v>0.54874614194131155</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4149,7 +4286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4187,7 +4324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -4225,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>0</v>
       </c>
@@ -4236,7 +4373,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -4253,7 +4390,7 @@
         <v>4.0918064501504169E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38">
         <f>STDEV(A$2,A$6,A$7,A$10)/SQRT(COUNT(A$2,A$6,A$7,A$10))</f>
         <v>1.0447399185554451E-3</v>
@@ -4267,7 +4404,7 @@
         <v>9.7749039349354682E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>0</v>
       </c>
@@ -4278,7 +4415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>4</v>
       </c>
@@ -4295,7 +4432,7 @@
         <v>2.6420759574462563E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C41">
         <f>STDEV(B$2,B$6,B$7,B$10)/SQRT(COUNT(B$2,B$6,B$7,B$10))</f>
         <v>7.5066653372385175E-3</v>
@@ -4309,7 +4446,7 @@
         <v>7.2439012414413602E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>0</v>
       </c>
@@ -4320,7 +4457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>5</v>
       </c>
@@ -4337,7 +4474,7 @@
         <v>281302308.30835921</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D44">
         <f>STDEV(C$2,C$6,C$7,C$10)/SQRT(COUNT(C$2,C$6,C$7,C$10))</f>
         <v>150436323.31557009</v>
@@ -4351,7 +4488,7 @@
         <v>119517745.49947689</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>0</v>
       </c>
@@ -4362,7 +4499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>6</v>
       </c>
@@ -4379,7 +4516,7 @@
         <v>17.162865937389306</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E47">
         <f>STDEV(D$2,D$6,D$7,D$10)/SQRT(COUNT(D$2,D$6,D$7,D$10))</f>
         <v>0.99200184873583563</v>
@@ -4393,7 +4530,7 @@
         <v>2.666105795193602</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
         <v>0</v>
       </c>
@@ -4404,7 +4541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
         <v>7</v>
       </c>
@@ -4421,7 +4558,7 @@
         <v>66.511511617894982</v>
       </c>
     </row>
-    <row r="50" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:13" x14ac:dyDescent="0.25">
       <c r="F50">
         <f>STDEV(E$2,E$6,E$7,E$10)/SQRT(COUNT(E$2,E$6,E$7,E$10))</f>
         <v>1.3615151309956437</v>
@@ -4435,7 +4572,7 @@
         <v>1.0334283378372413</v>
       </c>
     </row>
-    <row r="51" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:13" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
         <v>0</v>
       </c>
@@ -4446,7 +4583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:13" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
         <v>8</v>
       </c>
@@ -4463,7 +4600,7 @@
         <v>0.31865421713684139</v>
       </c>
     </row>
-    <row r="53" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:13" x14ac:dyDescent="0.25">
       <c r="G53">
         <f>STDEV(F$2,F$6,F$7,F$10)/SQRT(COUNT(F$2,F$6,F$7,F$10))</f>
         <v>1.5743495981404742E-2</v>
@@ -4477,7 +4614,7 @@
         <v>0.17590982786565229</v>
       </c>
     </row>
-    <row r="54" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H54" t="s">
         <v>0</v>
       </c>
@@ -4488,7 +4625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:13" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
         <v>9</v>
       </c>
@@ -4505,7 +4642,7 @@
         <v>1.0139519777450938E-2</v>
       </c>
     </row>
-    <row r="56" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H56">
         <f>STDEV(G$2,G$6,G$7,G$10)/SQRT(COUNT(G$2,G$6,G$7,G$10))</f>
         <v>0.71732924421815569</v>
@@ -4519,7 +4656,7 @@
         <v>6.421234854509128E-3</v>
       </c>
     </row>
-    <row r="57" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:13" x14ac:dyDescent="0.25">
       <c r="I57" t="s">
         <v>0</v>
       </c>
@@ -4530,7 +4667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:13" x14ac:dyDescent="0.25">
       <c r="H58" t="s">
         <v>10</v>
       </c>
@@ -4547,7 +4684,7 @@
         <v>2.4903235791122807E-3</v>
       </c>
     </row>
-    <row r="59" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:13" x14ac:dyDescent="0.25">
       <c r="I59">
         <f>STDEV(H$2,H$6,H$7,H$10)/SQRT(COUNT(H$2,H$6,H$7,H$10))</f>
         <v>1.4474098529035388E-7</v>
@@ -4561,7 +4698,7 @@
         <v>2.4903211112578764E-3</v>
       </c>
     </row>
-    <row r="60" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:13" x14ac:dyDescent="0.25">
       <c r="J60" t="s">
         <v>0</v>
       </c>
@@ -4572,7 +4709,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:13" x14ac:dyDescent="0.25">
       <c r="I61" t="s">
         <v>11</v>
       </c>
@@ -4589,7 +4726,7 @@
         <v>2.0254338466044231E-2</v>
       </c>
     </row>
-    <row r="62" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:13" x14ac:dyDescent="0.25">
       <c r="J62">
         <f>STDEV(I$2,I$6,I$7,I$10)/SQRT(COUNT(I$2,I$6,I$7,I$10))</f>
         <v>1.4433140442303676E-4</v>
@@ -4603,7 +4740,7 @@
         <v>3.3905745570573446E-4</v>
       </c>
     </row>
-    <row r="63" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:13" x14ac:dyDescent="0.25">
       <c r="K63" t="s">
         <v>0</v>
       </c>
@@ -4614,7 +4751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="5:13" x14ac:dyDescent="0.25">
       <c r="J64" t="s">
         <v>12</v>
       </c>
@@ -4631,7 +4768,7 @@
         <v>0.9908908327885434</v>
       </c>
     </row>
-    <row r="65" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K65">
         <f>STDEV(J$2,J$6,J$7,J$10)/SQRT(COUNT(J$2,J$6,J$7,J$10))</f>
         <v>6.4964877273083728E-3</v>
@@ -4645,7 +4782,7 @@
         <v>1.9805460745015197E-3</v>
       </c>
     </row>
-    <row r="66" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="11:16" x14ac:dyDescent="0.25">
       <c r="L66" t="s">
         <v>0</v>
       </c>
@@ -4656,7 +4793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="11:16" x14ac:dyDescent="0.25">
       <c r="K67" t="s">
         <v>13</v>
       </c>
@@ -4673,7 +4810,7 @@
         <v>0.89045016671936761</v>
       </c>
     </row>
-    <row r="68" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="11:16" x14ac:dyDescent="0.25">
       <c r="L68">
         <f>STDEV(K$2,K$6,K$7,K$10)/SQRT(COUNT(K$2,K$6,K$7,K$10))</f>
         <v>4.6562250904623494E-2</v>
@@ -4687,7 +4824,7 @@
         <v>7.1970014747289146E-2</v>
       </c>
     </row>
-    <row r="69" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="11:16" x14ac:dyDescent="0.25">
       <c r="M69" t="s">
         <v>0</v>
       </c>
@@ -4698,7 +4835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="11:16" x14ac:dyDescent="0.25">
       <c r="L70" t="s">
         <v>14</v>
       </c>
@@ -4715,7 +4852,7 @@
         <v>9.2996815108809333E-2</v>
       </c>
     </row>
-    <row r="71" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="11:16" x14ac:dyDescent="0.25">
       <c r="M71">
         <f>STDEV(L$2,L$6,L$7,L$10)/SQRT(COUNT(L$2,L$6,L$7,L$10))</f>
         <v>2.411341165056537E-2</v>
@@ -4729,7 +4866,7 @@
         <v>1.1100569339153378E-2</v>
       </c>
     </row>
-    <row r="72" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="11:16" x14ac:dyDescent="0.25">
       <c r="N72" t="s">
         <v>0</v>
       </c>
@@ -4740,7 +4877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="11:16" x14ac:dyDescent="0.25">
       <c r="M73" t="s">
         <v>15</v>
       </c>
@@ -4757,7 +4894,7 @@
         <v>0.275268451446878</v>
       </c>
     </row>
-    <row r="74" spans="11:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="11:16" x14ac:dyDescent="0.25">
       <c r="N74">
         <f>STDEV(M$2,M$6,M$7,M$10)/SQRT(COUNT(M$2,M$6,M$7,M$10))</f>
         <v>7.5908461419817039E-2</v>
@@ -4862,128 +4999,753 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C862FD-10AB-443F-A485-05C87B9A725E}">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CCEEE0D-57D3-4115-9DC8-BEFF121B996A}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30:N37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>3.4631571907257463E-2</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2">
+        <v>21.665856006620764</v>
+      </c>
+      <c r="F2">
+        <v>71.991112905571299</v>
+      </c>
+      <c r="G2">
+        <v>0.48964360836165388</v>
+      </c>
+      <c r="H2">
+        <v>0.98760204067091006</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2">
+        <v>2.0685325466676806E-2</v>
+      </c>
+      <c r="K2">
+        <v>0.9846208085278787</v>
+      </c>
+      <c r="L2">
+        <v>0.91205649327019656</v>
+      </c>
+      <c r="M2">
+        <v>0.11603488195925937</v>
+      </c>
+      <c r="N2">
+        <v>0.26593204270799609</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>3.407353040904397E-2</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>23.258065214118158</v>
+      </c>
+      <c r="F3">
+        <v>69.927538423613697</v>
+      </c>
+      <c r="G3">
+        <v>0.62467392697076818</v>
+      </c>
+      <c r="H3">
+        <v>0.7489205966313609</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3">
+        <v>2.0982889466742465E-2</v>
+      </c>
+      <c r="K3">
+        <v>0.99188467611926123</v>
+      </c>
+      <c r="L3">
+        <v>0.90338424524005434</v>
+      </c>
+      <c r="M3">
+        <v>8.7610595607189076E-2</v>
+      </c>
+      <c r="N3">
+        <v>0.27462705145025867</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="7">
-        <v>3.1891419103423092E-4</v>
-      </c>
-      <c r="C4" s="7">
-        <v>2.728623026116843E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="7">
-        <v>1.8056868879511054E-8</v>
-      </c>
-      <c r="C5" s="7">
-        <v>7.5830950699696309E-6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="7">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7">
+      <c r="B4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>2.6420759574462563E-2</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <v>17.162865937389306</v>
+      </c>
+      <c r="F4">
+        <v>66.511511617894982</v>
+      </c>
+      <c r="G4">
+        <v>0.31865421713684139</v>
+      </c>
+      <c r="H4">
+        <v>1.0139519777450938E-2</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4">
+        <v>2.0254338466044231E-2</v>
+      </c>
+      <c r="K4">
+        <v>0.9908908327885434</v>
+      </c>
+      <c r="L4">
+        <v>0.89045016671936761</v>
+      </c>
+      <c r="M4">
+        <v>9.2996815108809333E-2</v>
+      </c>
+      <c r="N4">
+        <v>0.275268451446878</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="7">
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>7.5066653372385175E-3</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7">
+        <v>0.99200184873583563</v>
+      </c>
+      <c r="F7">
+        <v>1.3615151309956437</v>
+      </c>
+      <c r="G7">
+        <v>1.5743495981404742E-2</v>
+      </c>
+      <c r="H7">
+        <v>0.71732924421815569</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7">
+        <v>4.6562250904623494E-2</v>
+      </c>
+      <c r="M7">
+        <v>2.411341165056537E-2</v>
+      </c>
+      <c r="N7">
+        <v>7.5908461419817039E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>5.4329446213610853E-3</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>3.5495295936658553</v>
+      </c>
+      <c r="F8">
+        <v>1.7684618034516078</v>
+      </c>
+      <c r="G8">
+        <v>2.8025073968266499E-2</v>
+      </c>
+      <c r="H8">
+        <v>0.54874614194131155</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8">
+        <v>3.5380735696335583E-2</v>
+      </c>
+      <c r="M8">
+        <v>8.4682250712293777E-3</v>
+      </c>
+      <c r="N8">
+        <v>6.3607515002683801E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9">
+        <v>2.666105795193602</v>
+      </c>
+      <c r="F9">
+        <v>1.0334283378372413</v>
+      </c>
+      <c r="G9">
+        <v>0.17590982786565229</v>
+      </c>
+      <c r="H9">
+        <v>6.421234854509128E-3</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9">
+        <v>7.1970014747289146E-2</v>
+      </c>
+      <c r="M9">
+        <v>1.1100569339153378E-2</v>
+      </c>
+      <c r="N9">
+        <v>0.10437371090759032</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="7">
-        <v>-2.1383818386594795</v>
-      </c>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="7">
-        <v>4.2746109123513287E-2</v>
-      </c>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="7">
-        <v>2.0150483733330233</v>
-      </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="7">
-        <v>8.5492218247026575E-2</v>
-      </c>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="8">
-        <v>2.570581835636315</v>
-      </c>
-      <c r="C13" s="8"/>
+      <c r="E22" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="str">
+        <f>IF(NOT(ISNUMBER(FIND("E",B2))),_xlfn.CONCAT(ROUND(B2,2), " ± ", ROUND(B7,2)),_xlfn.CONCAT(LEFT(B2,4),RIGHT(B2,4), " ± ",LEFT(B7,4),RIGHT(B7,4)))</f>
+        <v>1.58E-03 ± 1.04E-03</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" ref="C23:N23" si="0">IF(NOT(ISNUMBER(FIND("E",C2))),_xlfn.CONCAT(ROUND(C2,2), " ± ", ROUND(C7,2)),_xlfn.CONCAT(LEFT(C2,4),RIGHT(C2,4), " ± ",LEFT(C7,4),RIGHT(C7,4)))</f>
+        <v>0.03 ± 0.01</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>8.21E+08 ± 1.50E+08</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>21.67 ± 0.99</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>71.99 ± 1.36</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>0.49 ± 0.02</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>0.99 ± 0.72</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="0"/>
+        <v>4.47E-04 ± 1.45E-07</v>
+      </c>
+      <c r="J23" s="11" t="str">
+        <f>_xlfn.CONCAT(ROUND(J2,2)," ± ",J7)</f>
+        <v>0.02 ± 1.44E-04</v>
+      </c>
+      <c r="K23" s="11" t="str">
+        <f>_xlfn.CONCAT(ROUND(K2,2)," ± ",K7)</f>
+        <v>0.98 ± 6.50E-03</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="0"/>
+        <v>0.91 ± 0.05</v>
+      </c>
+      <c r="M23" t="str">
+        <f t="shared" si="0"/>
+        <v>0.12 ± 0.02</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="0"/>
+        <v>0.27 ± 0.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" ref="B24:N25" si="1">IF(NOT(ISNUMBER(FIND("E",B3))),_xlfn.CONCAT(ROUND(B3,2), " ± ", ROUND(B8,2)),_xlfn.CONCAT(LEFT(B3,4),RIGHT(B3,4), " ± ",LEFT(B8,4),RIGHT(B8,4)))</f>
+        <v>1.85E-03 ± 1.17E-03</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v>0.03 ± 0.01</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>8.85E+08 ± 1.33E+08</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>23.26 ± 3.55</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v>69.93 ± 1.77</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>0.62 ± 0.03</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="1"/>
+        <v>0.75 ± 0.55</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="1"/>
+        <v>1.88E-03 ± 1.64E-03</v>
+      </c>
+      <c r="J24" s="11" t="str">
+        <f t="shared" ref="J24:K25" si="2">_xlfn.CONCAT(ROUND(J3,2)," ± ",J8)</f>
+        <v>0.02 ± 8.32E-05</v>
+      </c>
+      <c r="K24" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>0.99 ± 1.45E-03</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="1"/>
+        <v>0.9 ± 0.04</v>
+      </c>
+      <c r="M24" t="str">
+        <f t="shared" si="1"/>
+        <v>0.09 ± 0.01</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="1"/>
+        <v>0.27 ± 0.06</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="1"/>
+        <v>4.09E-04 ± 9.77E-05</v>
+      </c>
+      <c r="C25" t="str">
+        <f>_xlfn.CONCAT(ROUND(C4,2)," ± ",C9)</f>
+        <v>0.03 ± 7.24E-05</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>2.81E+08 ± 1.20E+08</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>17.16 ± 2.67</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v>66.51 ± 1.03</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>0.32 ± 0.18</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="1"/>
+        <v>0.01 ± 0.01</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="1"/>
+        <v>2.49E-03 ± 2.49E-03</v>
+      </c>
+      <c r="J25" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>0.02 ± 3.39E-04</v>
+      </c>
+      <c r="K25" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>0.99 ± 1.98E-03</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="1"/>
+        <v>0.89 ± 0.07</v>
+      </c>
+      <c r="M25" t="str">
+        <f t="shared" si="1"/>
+        <v>0.09 ± 0.01</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="1"/>
+        <v>0.28 ± 0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" t="s">
+        <v>65</v>
+      </c>
+      <c r="H30" t="s">
+        <v>66</v>
+      </c>
+      <c r="M30" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" t="s">
+        <v>69</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N31" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G32" t="s">
+        <v>71</v>
+      </c>
+      <c r="H32" t="s">
+        <v>72</v>
+      </c>
+      <c r="L32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="N32" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M33" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="N33" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L34" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M34" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="N34" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L35" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M35" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="N35" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L36" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M36" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="N36" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="M37" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="N37" s="11" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4992,87 +5754,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D7CD97-2694-40DC-8F06-02B1972CDEB5}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>4.5806457239379913E-4</v>
-      </c>
-      <c r="B2" s="2">
-        <v>3.2228711889169465E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>3.0879274207964102E-4</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1.7498788269826546E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>1.8988525862925258E-4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3.8105221128828231E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
-        <v>5.2441769400202436E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
-        <v>6.3405155628034849E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
-        <v>4.7924853940454711E-4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5015D821-5D07-4755-AB9A-3C917D9CE095}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D94F58-F1C5-42AC-9C57-89D7EFD68CDA}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>2</v>
@@ -5081,40 +5779,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="7">
-        <v>8.4779244633254053E-3</v>
+        <v>4.0918064501504169E-4</v>
       </c>
       <c r="C4" s="7">
-        <v>1.0548675104176242</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1.8538458865264319E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="7">
-        <v>2.0285648946876051E-4</v>
+        <v>3.8219498774886763E-8</v>
       </c>
       <c r="C5" s="7">
-        <v>1.2914476403971797</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>8.2052527883177156E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
@@ -5123,7 +5821,7 @@
       </c>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
@@ -5132,25 +5830,25 @@
       </c>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="7">
-        <v>-2.2550824519745589</v>
+        <v>-1.231076260858188</v>
       </c>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="7">
-        <v>3.6902567688562399E-2</v>
+        <v>0.13651981198567228</v>
       </c>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
@@ -5159,16 +5857,16 @@
       </c>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="7">
-        <v>7.3805135377124798E-2</v>
+        <v>0.27303962397134457</v>
       </c>
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>27</v>
       </c>
@@ -5176,6 +5874,73 @@
         <v>2.570581835636315</v>
       </c>
       <c r="C13" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D7CD97-2694-40DC-8F06-02B1972CDEB5}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>5.1368495621184293E-4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2.8219214062879053E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>3.1190215825482111E-4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4.714109952254986E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1.8848694713137994E-4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>7.4960223764231736E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>6.2264851846212279E-4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.2207063174650723E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>2.5585370046212586E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>3.9688978895393006E-4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5183,16 +5948,144 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB333BE-D1CF-4B2F-90B0-1D0A12D03443}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1.0139519777450938E-2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.7489205966313609</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1.6492902822705144E-4</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.806733969772844</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="7">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="7">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="7">
+        <v>-1.3462153907947367</v>
+      </c>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.1180211698045624</v>
+      </c>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2.0150483733330233</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.2360423396091248</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2.570581835636315</v>
+      </c>
+      <c r="C13" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FBC4F0-A7F6-4632-A7BE-34442B5174FE}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -5200,43 +6093,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>3.4102255916542741E-4</v>
+        <v>1.0862895417044028E-7</v>
       </c>
       <c r="B2" s="2">
-        <v>6.6754770067435049E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.7619698660306608E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>2.4923758419106896E-2</v>
+        <v>2.6786842780739849E-2</v>
       </c>
       <c r="B3" s="2">
-        <v>1.7178910040439323E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.11412708907463566</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>1.6899241170389469E-4</v>
+        <v>4.196813171389801E-5</v>
       </c>
       <c r="B4" s="2">
-        <v>1.6910977041687847</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.4018200746017908</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1.3729159568395835E-2</v>
+      </c>
       <c r="B5" s="2">
-        <v>2.2278692972516283</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.90075717500536046</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>2.3031342775258441</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1.7323296211486903E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>4.0177224391649363E-2</v>
+        <v>2.1876246234585429E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to toolbox data, but decided to switch back to original algorithm
</commit_message>
<xml_diff>
--- a/LacTissue_hptoolbox.xlsx
+++ b/LacTissue_hptoolbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD640A53-1C2D-47F5-B6D4-5E8A2FDCF078}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA27733-5711-43A4-AD25-7E03C26D1A36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{20D85B12-9758-4F64-8529-8B10498F4544}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{20D85B12-9758-4F64-8529-8B10498F4544}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$25</c:f>
+              <c:f>Sheet1!$K$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -503,7 +503,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$L$26:$M$26</c:f>
+                <c:f>Sheet1!$L$27:$M$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -518,7 +518,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$L$26:$M$26</c:f>
+                <c:f>Sheet1!$L$27:$M$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -547,7 +547,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$24:$M$24</c:f>
+              <c:f>Sheet1!$L$25:$M$25</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -561,7 +561,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$25:$M$25</c:f>
+              <c:f>Sheet1!$L$26:$M$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -808,7 +808,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$31</c:f>
+              <c:f>Sheet1!$L$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -856,7 +856,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$M$32:$N$32</c:f>
+                <c:f>Sheet1!$M$33:$N$33</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -871,7 +871,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$M$32:$N$32</c:f>
+                <c:f>Sheet1!$M$33:$N$33</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
@@ -900,7 +900,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$M$30:$N$30</c:f>
+              <c:f>Sheet1!$M$31:$N$31</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -914,7 +914,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$31:$N$31</c:f>
+              <c:f>Sheet1!$M$32:$N$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -2233,13 +2233,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>12382</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>407670</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>44767</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2566,10 +2566,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B8402E-36A7-41FF-A256-45E2644B1621}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AB74"/>
+  <dimension ref="A1:AB75"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="S89" sqref="S89:X89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" activeCellId="13" sqref="K18 K16 K13 K12 K11 K10 K9 K8 K7 K6 K4 K3 K2 K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3675,1265 +3675,1291 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" ref="A19:A35" si="1">IF(OR(ABS(A2-T$5)&lt;=0.001*T$5,ABS(A2-T$6)&lt;=0.001*T$6),0,1)</f>
+      <c r="A19" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A1-T$5)&lt;=0.001*T$5,"Min",ABS(A1-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B19" s="11" t="str">
+        <f t="shared" ref="B19:I19" si="1">_xlfn.IFS(ABS(B1-U$5)&lt;=0.001*U$5,"Min",ABS(B1-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="D19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="E19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="F19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="G19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+      <c r="H19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>Max</v>
+      </c>
+      <c r="I19" s="11" t="str">
+        <f t="shared" si="1"/>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>_xlfn.IFS(ABS(A2-T$5)&lt;=0.001*T$5,"Min",ABS(A2-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B20" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B2-U$5)&lt;=0.001*U$5,"Min",ABS(B2-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C20" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C2-V$5)&lt;=0.001*V$5,"Min",ABS(C2-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D20" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D2-W$5)&lt;=0.001*W$5,"Min",ABS(D2-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E20" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E2-X$5)&lt;=0.001*X$5,"Min",ABS(E2-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F20" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F2-Y$5)&lt;=0.001*Y$5,"Min",ABS(F2-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G20" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G2-Z$5)&lt;=0.001*Z$5,"Min",ABS(G2-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H20" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H2-AA$5)&lt;=0.001*AA$5,"Min",ABS(H2-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I20" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I2-AB$5)&lt;=0.001*AB$5,"Min",ABS(I2-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A3-T$5)&lt;=0.001*T$5,"Min",ABS(A3-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B21" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B3-U$5)&lt;=0.001*U$5,"Min",ABS(B3-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C21" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C3-V$5)&lt;=0.001*V$5,"Min",ABS(C3-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D21" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D3-W$5)&lt;=0.001*W$5,"Min",ABS(D3-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E21" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E3-X$5)&lt;=0.001*X$5,"Min",ABS(E3-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F21" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F3-Y$5)&lt;=0.001*Y$5,"Min",ABS(F3-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G21" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G3-Z$5)&lt;=0.001*Z$5,"Min",ABS(G3-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H21" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H3-AA$5)&lt;=0.001*AA$5,"Min",ABS(H3-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I21" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I3-AB$5)&lt;=0.001*AB$5,"Min",ABS(I3-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A4-T$5)&lt;=0.001*T$5,"Min",ABS(A4-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B22" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B4-U$5)&lt;=0.001*U$5,"Min",ABS(B4-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C22" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C4-V$5)&lt;=0.001*V$5,"Min",ABS(C4-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D22" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D4-W$5)&lt;=0.001*W$5,"Min",ABS(D4-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E22" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E4-X$5)&lt;=0.001*X$5,"Min",ABS(E4-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F22" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F4-Y$5)&lt;=0.001*Y$5,"Min",ABS(F4-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G22" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G4-Z$5)&lt;=0.001*Z$5,"Min",ABS(G4-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H22" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H4-AA$5)&lt;=0.001*AA$5,"Min",ABS(H4-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I22" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I4-AB$5)&lt;=0.001*AB$5,"Min",ABS(I4-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A5-T$5)&lt;=0.001*T$5,"Min",ABS(A5-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B23" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B5-U$5)&lt;=0.001*U$5,"Min",ABS(B5-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C23" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C5-V$5)&lt;=0.001*V$5,"Min",ABS(C5-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D23" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D5-W$5)&lt;=0.001*W$5,"Min",ABS(D5-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E23" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E5-X$5)&lt;=0.001*X$5,"Min",ABS(E5-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F23" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F5-Y$5)&lt;=0.001*Y$5,"Min",ABS(F5-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G23" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G5-Z$5)&lt;=0.001*Z$5,"Min",ABS(G5-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H23" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H5-AA$5)&lt;=0.001*AA$5,"Min",ABS(H5-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I23" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I5-AB$5)&lt;=0.001*AB$5,"Min",ABS(I5-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A6-T$5)&lt;=0.001*T$5,"Min",ABS(A6-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B24" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B6-U$5)&lt;=0.001*U$5,"Min",ABS(B6-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C24" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C6-V$5)&lt;=0.001*V$5,"Min",ABS(C6-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D24" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D6-W$5)&lt;=0.001*W$5,"Min",ABS(D6-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E24" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E6-X$5)&lt;=0.001*X$5,"Min",ABS(E6-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F24" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F6-Y$5)&lt;=0.001*Y$5,"Min",ABS(F6-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G24" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G6-Z$5)&lt;=0.001*Z$5,"Min",ABS(G6-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H24" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H6-AA$5)&lt;=0.001*AA$5,"Min",ABS(H6-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I24" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I6-AB$5)&lt;=0.001*AB$5,"Min",ABS(I6-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A7-T$5)&lt;=0.001*T$5,"Min",ABS(A7-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B25" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B7-U$5)&lt;=0.001*U$5,"Min",ABS(B7-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C25" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C7-V$5)&lt;=0.001*V$5,"Min",ABS(C7-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D25" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D7-W$5)&lt;=0.001*W$5,"Min",ABS(D7-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E25" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E7-X$5)&lt;=0.001*X$5,"Min",ABS(E7-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F25" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F7-Y$5)&lt;=0.001*Y$5,"Min",ABS(F7-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G25" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G7-Z$5)&lt;=0.001*Z$5,"Min",ABS(G7-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H25" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H7-AA$5)&lt;=0.001*AA$5,"Min",ABS(H7-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I25" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I7-AB$5)&lt;=0.001*AB$5,"Min",ABS(I7-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="L25" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" t="s">
         <v>1</v>
       </c>
-      <c r="B19">
-        <f t="shared" ref="B19:F34" si="2">IF(OR(ABS(B2-U$5)&lt;=0.001*U$5,ABS(B2-U$6)&lt;=0.001*U$6),0,1)</f>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A8-T$5)&lt;=0.001*T$5,"Min",ABS(A8-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B26" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B8-U$5)&lt;=0.001*U$5,"Min",ABS(B8-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C26" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C8-V$5)&lt;=0.001*V$5,"Min",ABS(C8-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D26" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D8-W$5)&lt;=0.001*W$5,"Min",ABS(D8-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E26" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E8-X$5)&lt;=0.001*X$5,"Min",ABS(E8-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F26" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F8-Y$5)&lt;=0.001*Y$5,"Min",ABS(F8-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G26" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G8-Z$5)&lt;=0.001*Z$5,"Min",ABS(G8-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H26" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H8-AA$5)&lt;=0.001*AA$5,"Min",ABS(H8-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I26" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I8-AB$5)&lt;=0.001*AB$5,"Min",ABS(I8-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="K26" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26">
+        <v>4.0918064501504169E-4</v>
+      </c>
+      <c r="M26">
+        <v>1.8538458865264319E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A9-T$5)&lt;=0.001*T$5,"Min",ABS(A9-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B27" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B9-U$5)&lt;=0.001*U$5,"Min",ABS(B9-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C27" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C9-V$5)&lt;=0.001*V$5,"Min",ABS(C9-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D27" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D9-W$5)&lt;=0.001*W$5,"Min",ABS(D9-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E27" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E9-X$5)&lt;=0.001*X$5,"Min",ABS(E9-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F27" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F9-Y$5)&lt;=0.001*Y$5,"Min",ABS(F9-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G27" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G9-Z$5)&lt;=0.001*Z$5,"Min",ABS(G9-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H27" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H9-AA$5)&lt;=0.001*AA$5,"Min",ABS(H9-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I27" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I9-AB$5)&lt;=0.001*AB$5,"Min",ABS(I9-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Max</v>
+      </c>
+      <c r="L27">
+        <v>9.7749039349354682E-5</v>
+      </c>
+      <c r="M27">
+        <v>1.1694195702938643E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A10-T$5)&lt;=0.001*T$5,"Min",ABS(A10-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B28" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B10-U$5)&lt;=0.001*U$5,"Min",ABS(B10-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C28" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C10-V$5)&lt;=0.001*V$5,"Min",ABS(C10-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D28" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D10-W$5)&lt;=0.001*W$5,"Min",ABS(D10-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E28" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E10-X$5)&lt;=0.001*X$5,"Min",ABS(E10-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F28" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F10-Y$5)&lt;=0.001*Y$5,"Min",ABS(F10-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G28" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G10-Z$5)&lt;=0.001*Z$5,"Min",ABS(G10-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H28" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H10-AA$5)&lt;=0.001*AA$5,"Min",ABS(H10-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I28" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I10-AB$5)&lt;=0.001*AB$5,"Min",ABS(I10-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A11-T$5)&lt;=0.001*T$5,"Min",ABS(A11-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B29" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B11-U$5)&lt;=0.001*U$5,"Min",ABS(B11-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C29" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C11-V$5)&lt;=0.001*V$5,"Min",ABS(C11-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D29" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D11-W$5)&lt;=0.001*W$5,"Min",ABS(D11-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E29" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E11-X$5)&lt;=0.001*X$5,"Min",ABS(E11-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F29" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F11-Y$5)&lt;=0.001*Y$5,"Min",ABS(F11-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G29" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G11-Z$5)&lt;=0.001*Z$5,"Min",ABS(G11-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H29" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H11-AA$5)&lt;=0.001*AA$5,"Min",ABS(H11-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I29" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I11-AB$5)&lt;=0.001*AB$5,"Min",ABS(I11-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A12-T$5)&lt;=0.001*T$5,"Min",ABS(A12-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B30" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B12-U$5)&lt;=0.001*U$5,"Min",ABS(B12-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C30" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C12-V$5)&lt;=0.001*V$5,"Min",ABS(C12-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D30" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D12-W$5)&lt;=0.001*W$5,"Min",ABS(D12-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E30" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E12-X$5)&lt;=0.001*X$5,"Min",ABS(E12-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F30" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F12-Y$5)&lt;=0.001*Y$5,"Min",ABS(F12-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G30" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G12-Z$5)&lt;=0.001*Z$5,"Min",ABS(G12-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H30" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H12-AA$5)&lt;=0.001*AA$5,"Min",ABS(H12-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I30" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I12-AB$5)&lt;=0.001*AB$5,"Min",ABS(I12-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A13-T$5)&lt;=0.001*T$5,"Min",ABS(A13-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B31" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B13-U$5)&lt;=0.001*U$5,"Min",ABS(B13-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Min</v>
+      </c>
+      <c r="C31" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C13-V$5)&lt;=0.001*V$5,"Min",ABS(C13-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D31" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D13-W$5)&lt;=0.001*W$5,"Min",ABS(D13-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E31" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E13-X$5)&lt;=0.001*X$5,"Min",ABS(E13-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F31" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F13-Y$5)&lt;=0.001*Y$5,"Min",ABS(F13-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G31" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G13-Z$5)&lt;=0.001*Z$5,"Min",ABS(G13-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H31" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H13-AA$5)&lt;=0.001*AA$5,"Min",ABS(H13-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I31" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I13-AB$5)&lt;=0.001*AB$5,"Min",ABS(I13-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="M31" t="s">
+        <v>2</v>
+      </c>
+      <c r="N31" t="s">
         <v>1</v>
       </c>
-      <c r="C19">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A14-T$5)&lt;=0.001*T$5,"Min",ABS(A14-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B32" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B14-U$5)&lt;=0.001*U$5,"Min",ABS(B14-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C32" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C14-V$5)&lt;=0.001*V$5,"Min",ABS(C14-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D32" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D14-W$5)&lt;=0.001*W$5,"Min",ABS(D14-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E32" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E14-X$5)&lt;=0.001*X$5,"Min",ABS(E14-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F32" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F14-Y$5)&lt;=0.001*Y$5,"Min",ABS(F14-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G32" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G14-Z$5)&lt;=0.001*Z$5,"Min",ABS(G14-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H32" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H14-AA$5)&lt;=0.001*AA$5,"Min",ABS(H14-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I32" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I14-AB$5)&lt;=0.001*AB$5,"Min",ABS(I14-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="L32" t="s">
+        <v>28</v>
+      </c>
+      <c r="M32">
+        <v>1.0139519777450938E-2</v>
+      </c>
+      <c r="N32">
+        <v>0.7489205966313609</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A15-T$5)&lt;=0.001*T$5,"Min",ABS(A15-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B33" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B15-U$5)&lt;=0.001*U$5,"Min",ABS(B15-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C33" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C15-V$5)&lt;=0.001*V$5,"Min",ABS(C15-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D33" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D15-W$5)&lt;=0.001*W$5,"Min",ABS(D15-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E33" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E15-X$5)&lt;=0.001*X$5,"Min",ABS(E15-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F33" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F15-Y$5)&lt;=0.001*Y$5,"Min",ABS(F15-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G33" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G15-Z$5)&lt;=0.001*Z$5,"Min",ABS(G15-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H33" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H15-AA$5)&lt;=0.001*AA$5,"Min",ABS(H15-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I33" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I15-AB$5)&lt;=0.001*AB$5,"Min",ABS(I15-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="M33">
+        <v>6.421234854509128E-3</v>
+      </c>
+      <c r="N33">
+        <v>0.54874614194131155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A16-T$5)&lt;=0.001*T$5,"Min",ABS(A16-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B34" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B16-U$5)&lt;=0.001*U$5,"Min",ABS(B16-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Min</v>
+      </c>
+      <c r="C34" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C16-V$5)&lt;=0.001*V$5,"Min",ABS(C16-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D34" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D16-W$5)&lt;=0.001*W$5,"Min",ABS(D16-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E34" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E16-X$5)&lt;=0.001*X$5,"Min",ABS(E16-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F34" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F16-Y$5)&lt;=0.001*Y$5,"Min",ABS(F16-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G34" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G16-Z$5)&lt;=0.001*Z$5,"Min",ABS(G16-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H34" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H16-AA$5)&lt;=0.001*AA$5,"Min",ABS(H16-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I34" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I16-AB$5)&lt;=0.001*AB$5,"Min",ABS(I16-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A17-T$5)&lt;=0.001*T$5,"Min",ABS(A17-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B35" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B17-U$5)&lt;=0.001*U$5,"Min",ABS(B17-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C35" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C17-V$5)&lt;=0.001*V$5,"Min",ABS(C17-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D35" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D17-W$5)&lt;=0.001*W$5,"Min",ABS(D17-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E35" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E17-X$5)&lt;=0.001*X$5,"Min",ABS(E17-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F35" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F17-Y$5)&lt;=0.001*Y$5,"Min",ABS(F17-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="G35" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G17-Z$5)&lt;=0.001*Z$5,"Min",ABS(G17-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H35" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H17-AA$5)&lt;=0.001*AA$5,"Min",ABS(H17-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I35" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I17-AB$5)&lt;=0.001*AB$5,"Min",ABS(I17-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Max</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="str">
+        <f>_xlfn.IFS(ABS(A18-T$5)&lt;=0.001*T$5,"Min",ABS(A18-T$6)&lt;=0.001*T$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="B36" s="11" t="str">
+        <f>_xlfn.IFS(ABS(B18-U$5)&lt;=0.001*U$5,"Min",ABS(B18-U$6)&lt;=0.001*U$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="C36" s="11" t="str">
+        <f>_xlfn.IFS(ABS(C18-V$5)&lt;=0.001*V$5,"Min",ABS(C18-V$6)&lt;=0.001*V$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="D36" s="11" t="str">
+        <f>_xlfn.IFS(ABS(D18-W$5)&lt;=0.001*W$5,"Min",ABS(D18-W$6)&lt;=0.001*W$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="E36" s="11" t="str">
+        <f>_xlfn.IFS(ABS(E18-X$5)&lt;=0.001*X$5,"Min",ABS(E18-X$6)&lt;=0.001*X$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="F36" s="11" t="str">
+        <f>_xlfn.IFS(ABS(F18-Y$5)&lt;=0.001*Y$5,"Min",ABS(F18-Y$6)&lt;=0.001*Y$6,"Max",TRUE,"Ok")</f>
+        <v>Min</v>
+      </c>
+      <c r="G36" s="11" t="str">
+        <f>_xlfn.IFS(ABS(G18-Z$5)&lt;=0.001*Z$5,"Min",ABS(G18-Z$6)&lt;=0.001*Z$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="H36" s="11" t="str">
+        <f>_xlfn.IFS(ABS(H18-AA$5)&lt;=0.001*AA$5,"Min",ABS(H18-AA$6)&lt;=0.001*AA$6,"Max",TRUE,"Ok")</f>
+        <v>Ok</v>
+      </c>
+      <c r="I36" s="11" t="str">
+        <f>_xlfn.IFS(ABS(I18-AB$5)&lt;=0.001*AB$5,"Min",ABS(I18-AB$6)&lt;=0.001*AB$6,"Max",TRUE,"Ok")</f>
+        <v>Min</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
         <v>1</v>
       </c>
-      <c r="D19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <f t="shared" ref="G19:G35" si="3">IF(OR(ABS(G2-Z$5)&lt;=0.001*Z$5,ABS(G2-Z$6)&lt;=0.001*Z$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <f t="shared" ref="H19:H35" si="4">IF(OR(ABS(H2-AA$5)&lt;=0.001*AA$5,ABS(H2-AA$6)&lt;=0.001*AA$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <f t="shared" ref="I19:I35" si="5">IF(OR(ABS(I2-AB$5)&lt;=0.001*AB$5,ABS(I2-AB$6)&lt;=0.001*AB$6),0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="D37" t="s">
         <v>2</v>
       </c>
-      <c r="M24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="K25" t="s">
-        <v>16</v>
-      </c>
-      <c r="L25">
-        <v>4.0918064501504169E-4</v>
-      </c>
-      <c r="M25">
-        <v>1.8538458865264319E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>9.7749039349354682E-5</v>
-      </c>
-      <c r="M26">
-        <v>1.1694195702938643E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B30">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="M30" t="s">
-        <v>2</v>
-      </c>
-      <c r="N30" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="L31" t="s">
-        <v>28</v>
-      </c>
-      <c r="M31">
-        <v>1.0139519777450938E-2</v>
-      </c>
-      <c r="N31">
-        <v>0.7489205966313609</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="M32">
-        <v>6.421234854509128E-3</v>
-      </c>
-      <c r="N32">
-        <v>0.54874614194131155</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <f t="shared" ref="B35" si="6">IF(OR(ABS(B18-U$5)&lt;=0.001*U$5,ABS(B18-U$6)&lt;=0.001*U$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="C35">
-        <f t="shared" ref="C35" si="7">IF(OR(ABS(C18-V$5)&lt;=0.001*V$5,ABS(C18-V$6)&lt;=0.001*V$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <f t="shared" ref="D35" si="8">IF(OR(ABS(D18-W$5)&lt;=0.001*W$5,ABS(D18-W$6)&lt;=0.001*W$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <f t="shared" ref="E35" si="9">IF(OR(ABS(E18-X$5)&lt;=0.001*X$5,ABS(E18-X$6)&lt;=0.001*X$6),0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <f t="shared" ref="F35" si="10">IF(OR(ABS(F18-Y$5)&lt;=0.001*Y$5,ABS(F18-Y$6)&lt;=0.001*Y$6),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>3</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <f>AVERAGE(A$2,A$4,A$6,A$7,A$10)</f>
         <v>1.5756130817148738E-3</v>
       </c>
-      <c r="C37">
+      <c r="C38">
         <f>AVERAGE(A$1,A$3,A$8,A$9,A$11,A$12)</f>
         <v>1.8538458865264319E-3</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <f>AVERAGE(A$13,A$15,A$16,A$18)</f>
         <v>4.0918064501504169E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B38">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B39">
         <f>STDEV(A$2,A$6,A$7,A$10)/SQRT(COUNT(A$2,A$6,A$7,A$10))</f>
         <v>1.0447399185554451E-3</v>
       </c>
-      <c r="C38">
+      <c r="C39">
         <f>STDEV(A$1,A$3,A$8,A$9,A$11,A$12)/SQRT(COUNT(A$1,A$3,A$8,A$9,A$11,A$12))</f>
         <v>1.1694195702938643E-3</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <f>STDEV(A$13,A$15,A$16,A$18)/SQRT(COUNT(A$13,A$15,A$16,A$18))</f>
         <v>9.7749039349354682E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
         <v>1</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>4</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <f>AVERAGE(B$2,B$4,B$6,B$7,B$10)</f>
         <v>3.4631571907257463E-2</v>
       </c>
-      <c r="D40">
+      <c r="D41">
         <f>AVERAGE(B$1,B$3,B$8,B$9,B$11,B$12)</f>
         <v>3.407353040904397E-2</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <f>AVERAGE(B$13,B$15,B$16,B$18)</f>
         <v>2.6420759574462563E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C41">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C42">
         <f>STDEV(B$2,B$6,B$7,B$10)/SQRT(COUNT(B$2,B$6,B$7,B$10))</f>
         <v>7.5066653372385175E-3</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <f>STDEV(B$1,B$3,B$8,B$9,B$11,B$12)/SQRT(COUNT(B$1,B$3,B$8,B$9,B$11,B$12))</f>
         <v>5.4329446213610853E-3</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <f>STDEV(B$13,B$15,B$16,B$18)/SQRT(COUNT(B$13,B$15,B$16,B$18))</f>
         <v>7.2439012414413602E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
         <v>1</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F43" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>5</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <f>AVERAGE(C$2,C$4,C$6,C$7,C$10)</f>
         <v>821016643.60751045</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <f>AVERAGE(C$1,C$3,C$8,C$9,C$11,C$12)</f>
         <v>884795162.76478398</v>
       </c>
-      <c r="F43">
+      <c r="F44">
         <f>AVERAGE(C$13,C$15,C$16,C$18)</f>
         <v>281302308.30835921</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D44">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D45">
         <f>STDEV(C$2,C$6,C$7,C$10)/SQRT(COUNT(C$2,C$6,C$7,C$10))</f>
         <v>150436323.31557009</v>
       </c>
-      <c r="E44">
+      <c r="E45">
         <f>STDEV(C$1,C$3,C$8,C$9,C$11,C$12)/SQRT(COUNT(C$1,C$3,C$8,C$9,C$11,C$12))</f>
         <v>132589557.77586628</v>
       </c>
-      <c r="F44">
+      <c r="F45">
         <f>STDEV(C$13,C$15,C$16,C$18)/SQRT(COUNT(C$13,C$15,C$16,C$18))</f>
         <v>119517745.49947689</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E45" t="s">
-        <v>0</v>
-      </c>
-      <c r="F45" t="s">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
         <v>1</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G46" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
         <v>6</v>
       </c>
-      <c r="E46">
+      <c r="E47">
         <f>AVERAGE(D$2,D$4,D$6,D$7,D$10)</f>
         <v>21.665856006620764</v>
       </c>
-      <c r="F46">
+      <c r="F47">
         <f>AVERAGE(D$1,D$3,D$8,D$9,D$11,D$12)</f>
         <v>23.258065214118158</v>
       </c>
-      <c r="G46">
+      <c r="G47">
         <f>AVERAGE(D$13,D$15,D$16,D$18)</f>
         <v>17.162865937389306</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E47">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E48">
         <f>STDEV(D$2,D$6,D$7,D$10)/SQRT(COUNT(D$2,D$6,D$7,D$10))</f>
         <v>0.99200184873583563</v>
       </c>
-      <c r="F47">
+      <c r="F48">
         <f>STDEV(D$1,D$3,D$8,D$9,D$11,D$12)/SQRT(COUNT(D$1,D$3,D$8,D$9,D$11,D$12))</f>
         <v>3.5495295936658553</v>
       </c>
-      <c r="G47">
+      <c r="G48">
         <f>STDEV(D$13,D$15,D$16,D$18)/SQRT(COUNT(D$13,D$15,D$16,D$18))</f>
         <v>2.666105795193602</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F48" t="s">
-        <v>0</v>
-      </c>
-      <c r="G48" t="s">
+    <row r="49" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
         <v>1</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H49" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E49" t="s">
+    <row r="50" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
         <v>7</v>
       </c>
-      <c r="F49">
+      <c r="F50">
         <f>AVERAGE(E$2,E$4,E$6,E$7,E$10)</f>
         <v>71.991112905571299</v>
       </c>
-      <c r="G49">
+      <c r="G50">
         <f>AVERAGE(E$1,E$3,E$8,E$9,E$11,E$12)</f>
         <v>69.927538423613697</v>
       </c>
-      <c r="H49">
+      <c r="H50">
         <f>AVERAGE(E$13,E$15,E$16,E$18)</f>
         <v>66.511511617894982</v>
       </c>
     </row>
-    <row r="50" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="F50">
+    <row r="51" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="F51">
         <f>STDEV(E$2,E$6,E$7,E$10)/SQRT(COUNT(E$2,E$6,E$7,E$10))</f>
         <v>1.3615151309956437</v>
       </c>
-      <c r="G50">
+      <c r="G51">
         <f>STDEV(E$1,E$3,E$8,E$9,E$11,E$12)/SQRT(COUNT(E$1,E$3,E$8,E$9,E$11,E$12))</f>
         <v>1.7684618034516078</v>
       </c>
-      <c r="H50">
+      <c r="H51">
         <f>STDEV(E$13,E$15,E$16,E$18)/SQRT(COUNT(E$13,E$15,E$16,E$18))</f>
         <v>1.0334283378372413</v>
       </c>
     </row>
-    <row r="51" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="G51" t="s">
-        <v>0</v>
-      </c>
-      <c r="H51" t="s">
+    <row r="52" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>0</v>
+      </c>
+      <c r="H52" t="s">
         <v>1</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I52" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="F52" t="s">
+    <row r="53" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
         <v>8</v>
       </c>
-      <c r="G52">
+      <c r="G53">
         <f>AVERAGE(F$2,F$4,F$6,F$7,F$10)</f>
         <v>0.48964360836165388</v>
       </c>
-      <c r="H52">
+      <c r="H53">
         <f>AVERAGE(F$1,F$3,F$8,F$9,F$11,F$12)</f>
         <v>0.62467392697076818</v>
       </c>
-      <c r="I52">
+      <c r="I53">
         <f>AVERAGE(F$13,F$15,F$16,F$18)</f>
         <v>0.31865421713684139</v>
       </c>
     </row>
-    <row r="53" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="G53">
+    <row r="54" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G54">
         <f>STDEV(F$2,F$6,F$7,F$10)/SQRT(COUNT(F$2,F$6,F$7,F$10))</f>
         <v>1.5743495981404742E-2</v>
       </c>
-      <c r="H53">
+      <c r="H54">
         <f>STDEV(F$1,F$3,F$8,F$9,F$11,F$12)/SQRT(COUNT(F$1,F$3,F$8,F$9,F$11,F$12))</f>
         <v>2.8025073968266499E-2</v>
       </c>
-      <c r="I53">
+      <c r="I54">
         <f>STDEV(F$13,F$15,F$16,F$18)/SQRT(COUNT(F$13,F$15,F$16,F$18))</f>
         <v>0.17590982786565229</v>
       </c>
     </row>
-    <row r="54" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="H54" t="s">
-        <v>0</v>
-      </c>
-      <c r="I54" t="s">
+    <row r="55" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
         <v>1</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J55" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="G55" t="s">
+    <row r="56" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
         <v>9</v>
       </c>
-      <c r="H55">
+      <c r="H56">
         <f>AVERAGE(G$2,G$4,G$6,G$7,G$10)</f>
         <v>0.98760204067091006</v>
       </c>
-      <c r="I55">
+      <c r="I56">
         <f>AVERAGE(G$1,G$3,G$8,G$9,G$11,G$12)</f>
         <v>0.7489205966313609</v>
       </c>
-      <c r="J55">
+      <c r="J56">
         <f>AVERAGE(G$13,G$15,G$16,G$18)</f>
         <v>1.0139519777450938E-2</v>
       </c>
     </row>
-    <row r="56" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="H56">
+    <row r="57" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H57">
         <f>STDEV(G$2,G$6,G$7,G$10)/SQRT(COUNT(G$2,G$6,G$7,G$10))</f>
         <v>0.71732924421815569</v>
       </c>
-      <c r="I56">
+      <c r="I57">
         <f>STDEV(G$1,G$3,G$8,G$9,G$11,G$12)/SQRT(COUNT(G$1,G$3,G$8,G$9,G$11,G$12))</f>
         <v>0.54874614194131155</v>
       </c>
-      <c r="J56">
+      <c r="J57">
         <f>STDEV(G$13,G$15,G$16,G$18)/SQRT(COUNT(G$13,G$15,G$16,G$18))</f>
         <v>6.421234854509128E-3</v>
       </c>
     </row>
-    <row r="57" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="I57" t="s">
-        <v>0</v>
-      </c>
-      <c r="J57" t="s">
+    <row r="58" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="I58" t="s">
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
         <v>1</v>
       </c>
-      <c r="K57" t="s">
+      <c r="K58" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="H58" t="s">
+    <row r="59" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
         <v>10</v>
       </c>
-      <c r="I58">
+      <c r="I59">
         <f>AVERAGE(H$2,H$4,H$6,H$7,H$10)</f>
         <v>4.4737202209835106E-4</v>
       </c>
-      <c r="J58">
+      <c r="J59">
         <f>AVERAGE(H$1,H$3,H$8,H$9,H$11,H$12)</f>
         <v>1.8813807020430105E-3</v>
       </c>
-      <c r="K58">
+      <c r="K59">
         <f>AVERAGE(H$13,H$15,H$16,H$18)</f>
         <v>2.4903235791122807E-3</v>
       </c>
     </row>
-    <row r="59" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="I59">
+    <row r="60" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="I60">
         <f>STDEV(H$2,H$6,H$7,H$10)/SQRT(COUNT(H$2,H$6,H$7,H$10))</f>
         <v>1.4474098529035388E-7</v>
       </c>
-      <c r="J59">
+      <c r="J60">
         <f>STDEV(H$1,H$3,H$8,H$9,H$11,H$12)/SQRT(COUNT(H$1,H$3,H$8,H$9,H$11,H$12))</f>
         <v>1.6367988425098196E-3</v>
       </c>
-      <c r="K59">
+      <c r="K60">
         <f>STDEV(H$13,H$15,H$16,H$18)/SQRT(COUNT(H$13,H$15,H$16,H$18))</f>
         <v>2.4903211112578764E-3</v>
       </c>
     </row>
-    <row r="60" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="J60" t="s">
-        <v>0</v>
-      </c>
-      <c r="K60" t="s">
+    <row r="61" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>0</v>
+      </c>
+      <c r="K61" t="s">
         <v>1</v>
       </c>
-      <c r="L60" t="s">
+      <c r="L61" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="I61" t="s">
+    <row r="62" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="I62" t="s">
         <v>11</v>
       </c>
-      <c r="J61">
+      <c r="J62">
         <f>AVERAGE(I$2,I$4,I$6,I$7,I$10)</f>
         <v>2.0685325466676806E-2</v>
       </c>
-      <c r="K61">
+      <c r="K62">
         <f>AVERAGE(I$1,I$3,I$8,I$9,I$11,I$12)</f>
         <v>2.0982889466742465E-2</v>
       </c>
-      <c r="L61">
+      <c r="L62">
         <f>AVERAGE(I$13,I$15,I$16,I$18)</f>
         <v>2.0254338466044231E-2</v>
       </c>
     </row>
-    <row r="62" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="J62">
+    <row r="63" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="J63">
         <f>STDEV(I$2,I$6,I$7,I$10)/SQRT(COUNT(I$2,I$6,I$7,I$10))</f>
         <v>1.4433140442303676E-4</v>
       </c>
-      <c r="K62">
+      <c r="K63">
         <f>STDEV(I$1,I$3,I$8,I$9,I$11,I$12)/SQRT(COUNT(I$1,I$3,I$8,I$9,I$11,I$12))</f>
         <v>8.3232065221440667E-5</v>
       </c>
-      <c r="L62">
+      <c r="L63">
         <f>STDEV(I$13,I$15,I$16,I$18)/SQRT(COUNT(I$13,I$15,I$16,I$18))</f>
         <v>3.3905745570573446E-4</v>
       </c>
     </row>
-    <row r="63" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="K63" t="s">
-        <v>0</v>
-      </c>
-      <c r="L63" t="s">
+    <row r="64" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="K64" t="s">
+        <v>0</v>
+      </c>
+      <c r="L64" t="s">
         <v>1</v>
       </c>
-      <c r="M63" t="s">
+      <c r="M64" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="J64" t="s">
+    <row r="65" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
         <v>12</v>
       </c>
-      <c r="K64">
+      <c r="K65">
         <f>AVERAGE(J$2,J$4,J$6,J$7,J$10)</f>
         <v>0.9846208085278787</v>
       </c>
-      <c r="L64">
+      <c r="L65">
         <f>AVERAGE(J$1,J$3,J$8,J$9,J$11,J$12)</f>
         <v>0.99188467611926123</v>
       </c>
-      <c r="M64">
+      <c r="M65">
         <f>AVERAGE(J$13,J$15,J$16,J$18)</f>
         <v>0.9908908327885434</v>
       </c>
     </row>
-    <row r="65" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K65">
+    <row r="66" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="K66">
         <f>STDEV(J$2,J$6,J$7,J$10)/SQRT(COUNT(J$2,J$6,J$7,J$10))</f>
         <v>6.4964877273083728E-3</v>
       </c>
-      <c r="L65">
+      <c r="L66">
         <f>STDEV(J$1,J$3,J$8,J$9,J$11,J$12)/SQRT(COUNT(J$1,J$3,J$8,J$9,J$11,J$12))</f>
         <v>1.4495210884977621E-3</v>
       </c>
-      <c r="M65">
+      <c r="M66">
         <f>STDEV(J$13,J$15,J$16,J$18)/SQRT(COUNT(J$13,J$15,J$16,J$18))</f>
         <v>1.9805460745015197E-3</v>
       </c>
     </row>
-    <row r="66" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="L66" t="s">
-        <v>0</v>
-      </c>
-      <c r="M66" t="s">
+    <row r="67" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="L67" t="s">
+        <v>0</v>
+      </c>
+      <c r="M67" t="s">
         <v>1</v>
       </c>
-      <c r="N66" t="s">
+      <c r="N67" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K67" t="s">
+    <row r="68" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="K68" t="s">
         <v>13</v>
       </c>
-      <c r="L67">
+      <c r="L68">
         <f>AVERAGE(K$2,K$4,K$6,K$7,K$10)</f>
         <v>0.91205649327019656</v>
       </c>
-      <c r="M67">
+      <c r="M68">
         <f>AVERAGE(K$1,K$3,K$8,K$9,K$11,K$12)</f>
         <v>0.90338424524005434</v>
       </c>
-      <c r="N67">
+      <c r="N68">
         <f>AVERAGE(K$13,K$15,K$16,K$18)</f>
         <v>0.89045016671936761</v>
       </c>
     </row>
-    <row r="68" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="L68">
+    <row r="69" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="L69">
         <f>STDEV(K$2,K$6,K$7,K$10)/SQRT(COUNT(K$2,K$6,K$7,K$10))</f>
         <v>4.6562250904623494E-2</v>
       </c>
-      <c r="M68">
+      <c r="M69">
         <f>STDEV(K$1,K$3,K$8,K$9,K$11,K$12)/SQRT(COUNT(K$1,K$3,K$8,K$9,K$11,K$12))</f>
         <v>3.5380735696335583E-2</v>
       </c>
-      <c r="N68">
+      <c r="N69">
         <f>STDEV(K$13,K$15,K$16,K$18)/SQRT(COUNT(K$13,K$15,K$16,K$18))</f>
         <v>7.1970014747289146E-2</v>
       </c>
     </row>
-    <row r="69" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="M69" t="s">
-        <v>0</v>
-      </c>
-      <c r="N69" t="s">
+    <row r="70" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="M70" t="s">
+        <v>0</v>
+      </c>
+      <c r="N70" t="s">
         <v>1</v>
       </c>
-      <c r="O69" t="s">
+      <c r="O70" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="L70" t="s">
+    <row r="71" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="L71" t="s">
         <v>14</v>
       </c>
-      <c r="M70">
+      <c r="M71">
         <f>AVERAGE(L$2,L$4,L$6,L$7,L$10)</f>
         <v>0.11603488195925937</v>
       </c>
-      <c r="N70">
+      <c r="N71">
         <f>AVERAGE(L$1,L$3,L$8,L$9,L$11,L$12)</f>
         <v>8.7610595607189076E-2</v>
       </c>
-      <c r="O70">
+      <c r="O71">
         <f>AVERAGE(L$13,L$15,L$16,L$18)</f>
         <v>9.2996815108809333E-2</v>
       </c>
     </row>
-    <row r="71" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="M71">
+    <row r="72" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="M72">
         <f>STDEV(L$2,L$6,L$7,L$10)/SQRT(COUNT(L$2,L$6,L$7,L$10))</f>
         <v>2.411341165056537E-2</v>
       </c>
-      <c r="N71">
+      <c r="N72">
         <f>STDEV(L$1,L$3,L$8,L$9,L$11,L$12)/SQRT(COUNT(L$1,L$3,L$8,L$9,L$11,L$12))</f>
         <v>8.4682250712293777E-3</v>
       </c>
-      <c r="O71">
+      <c r="O72">
         <f>STDEV(L$13,L$15,L$16,L$18)/SQRT(COUNT(L$13,L$15,L$16,L$18))</f>
         <v>1.1100569339153378E-2</v>
       </c>
     </row>
-    <row r="72" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="N72" t="s">
-        <v>0</v>
-      </c>
-      <c r="O72" t="s">
+    <row r="73" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="N73" t="s">
+        <v>0</v>
+      </c>
+      <c r="O73" t="s">
         <v>1</v>
       </c>
-      <c r="P72" t="s">
+      <c r="P73" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="M73" t="s">
+    <row r="74" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="M74" t="s">
         <v>15</v>
       </c>
-      <c r="N73">
+      <c r="N74">
         <f>AVERAGE(M$2,M$4,M$6,M$7,M$10)</f>
         <v>0.26593204270799609</v>
       </c>
-      <c r="O73">
+      <c r="O74">
         <f>AVERAGE(M$1,M$3,M$8,M$9,M$11,M$12)</f>
         <v>0.27462705145025867</v>
       </c>
-      <c r="P73">
+      <c r="P74">
         <f>AVERAGE(M$13,M$15,M$16,M$18)</f>
         <v>0.275268451446878</v>
       </c>
     </row>
-    <row r="74" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="N74">
+    <row r="75" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="N75">
         <f>STDEV(M$2,M$6,M$7,M$10)/SQRT(COUNT(M$2,M$6,M$7,M$10))</f>
         <v>7.5908461419817039E-2</v>
       </c>
-      <c r="O74">
+      <c r="O75">
         <f>STDEV(M$1,M$3,M$8,M$9,M$11,M$12)/SQRT(COUNT(M$1,M$3,M$8,M$9,M$11,M$12))</f>
         <v>6.3607515002683801E-2</v>
       </c>
-      <c r="P74">
+      <c r="P75">
         <f>STDEV(M$13,M$15,M$16,M$18)/SQRT(COUNT(M$13,M$15,M$16,M$18))</f>
         <v>0.10437371090759032</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L1:L17">
+  <conditionalFormatting sqref="A19:I36">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M17">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19:I35">
+  <conditionalFormatting sqref="A19:I36">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -4945,8 +4971,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N18">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="L1:L4 L6:L13 L15:L16 L18">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4957,32 +4983,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19:I35">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L18">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M1:M18">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="M1:M4 M6:M13 M15:M16 M18">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5003,8 +5005,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30:N37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>